<commit_message>
test 1 nogif stats
</commit_message>
<xml_diff>
--- a/test1-input-optimization/filesize.xlsx
+++ b/test1-input-optimization/filesize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="307">
   <si>
     <t>Filename</t>
   </si>
@@ -937,6 +937,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>NOGIF MEAN</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1045,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1090,8 +1093,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1104,8 +1109,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1129,6 +1135,7 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1152,6 +1159,7 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1481,11 +1489,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A144" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E160" sqref="E160"/>
+      <pane ySplit="2" topLeftCell="A126" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6041,6 +6049,21 @@
         <v>83843</v>
       </c>
     </row>
+    <row r="153" spans="1:9" s="1" customFormat="1">
+      <c r="A153" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="B153" s="2"/>
+      <c r="C153" s="8">
+        <f>AVERAGE(C3:C38,C48:C87,C97:C136,C146:C149)</f>
+        <v>344250.61666666664</v>
+      </c>
+      <c r="E153" s="8">
+        <f>AVERAGE(E3:E38,E48:E87,E97:E136,E146:E149)</f>
+        <v>344949.30833333335</v>
+      </c>
+      <c r="I153" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>